<commit_message>
Update Fineco trasformer to the new file format (data begins one row earlier)
</commit_message>
<xml_diff>
--- a/tests/Fixtures/movimenti-fineco-test-contabilizzati.xlsx
+++ b/tests/Fixtures/movimenti-fineco-test-contabilizzati.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francesco/francesco/sviluppo/progetti/ynab-transformer/tests/Fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE6D66C-9946-F64D-873B-C2EE2E808ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973956C5-5DE5-5E4D-8204-1BBFFD5E1988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4040" yWindow="5980" windowWidth="22760" windowHeight="13400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -114,8 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -459,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -475,111 +474,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>9</v>
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>-11.59</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1">
-        <v>-11.59</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="A9" s="3">
+        <v>44439</v>
+      </c>
+      <c r="C9">
+        <v>-15.56</v>
+      </c>
+      <c r="D9" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1">
-      <c r="A10" s="4">
-        <v>44439</v>
-      </c>
-      <c r="C10" s="1">
-        <v>-15.56</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="E12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Handle updated Fineco format
</commit_message>
<xml_diff>
--- a/tests/Fixtures/movimenti-fineco-test-contabilizzati.xlsx
+++ b/tests/Fixtures/movimenti-fineco-test-contabilizzati.xlsx
@@ -2,36 +2,45 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/tmp/cleaned-fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francesco/francesco/sviluppo/progetti/ynab-transformer/tests/Fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202A88AD-3C04-1C4C-80FD-2E321E3057FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE5706BA-AE6C-3143-98D4-6D4D64DB834F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19340" yWindow="7960" windowWidth="22760" windowHeight="13400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="7780" windowWidth="22840" windowHeight="19920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Organization" sheetId="1" r:id="rId1"/>
+    <sheet name="Movimenti" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Periodo Dal: 2021-08-01 Al: 2021-08-22</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
+  <si>
+    <t>Periodo Dal: 05/06/2025 Al: 03/09/2025</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Nota: Per le carte di credito la data valuta è quella di registrazione contabile dell'operazione e non quella di addebito sul conto corrente.</t>
+  </si>
+  <si>
+    <t>Nota: Per le carte di debito la data operazione non è quella in cui il pagamento è stato effettuato ed autorizzato (pari alla data valuta) ma il giorno in cui il movimento è stato contabilizzato.</t>
   </si>
   <si>
     <t>Risultati Ricerca</t>
   </si>
   <si>
-    <t>Data</t>
+    <t>Data_Operazione</t>
+  </si>
+  <si>
+    <t>Data_Valuta</t>
   </si>
   <si>
     <t>Entrate</t>
@@ -43,53 +52,44 @@
     <t>Descrizione</t>
   </si>
   <si>
-    <t>Descrizione Completa</t>
+    <t>Descrizione_Completa</t>
   </si>
   <si>
     <t>Stato</t>
   </si>
   <si>
-    <t>Moneymap</t>
-  </si>
-  <si>
-    <t>21/08/2021</t>
-  </si>
-  <si>
-    <t>VISA DEBIT</t>
+    <t>Contabilizzato</t>
+  </si>
+  <si>
+    <t>Pagamento Visa Debit</t>
+  </si>
+  <si>
+    <t>Autorizzato</t>
+  </si>
+  <si>
+    <t>Conto Corrente: 0002921637</t>
+  </si>
+  <si>
+    <t>Intestazione Conto Corrente: HOMER SIMPSON</t>
   </si>
   <si>
     <t>AMZN Mktp IT</t>
-  </si>
-  <si>
-    <t>Autorizzato</t>
-  </si>
-  <si>
-    <t>Contabilizzato</t>
-  </si>
-  <si>
-    <t>Conto Corrente: 0003826218</t>
-  </si>
-  <si>
-    <t>Intestazione Conto Corrente: HOMER SIMPSON</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -114,11 +114,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,108 +457,1146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
-    <col min="6" max="6" width="14.5" customWidth="1"/>
-    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="25.83203125" customWidth="1"/>
+    <col min="5" max="5" width="50.83203125" customWidth="1"/>
+    <col min="6" max="7" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="1" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="D10" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="E10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="F10" t="s">
         <v>10</v>
       </c>
-      <c r="C8">
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>44429</v>
+      </c>
+      <c r="B11" s="1">
+        <v>44429</v>
+      </c>
+      <c r="D11">
         <v>-11.59</v>
       </c>
-      <c r="D8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="E11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="G11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>44439</v>
       </c>
-      <c r="C9">
+      <c r="B12" s="1">
+        <v>44439</v>
+      </c>
+      <c r="D12">
         <v>-15.56</v>
       </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="1"/>
+      <c r="B119" s="1"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="1"/>
+      <c r="B120" s="1"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="1"/>
+      <c r="B121" s="1"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="1"/>
+      <c r="B140" s="1"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="1"/>
+      <c r="B141" s="1"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="1"/>
+      <c r="B142" s="1"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="1"/>
+      <c r="B143" s="1"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="1"/>
+      <c r="B144" s="1"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="1"/>
+      <c r="B145" s="1"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="1"/>
+      <c r="B147" s="1"/>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="1"/>
+      <c r="B148" s="1"/>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="1"/>
+      <c r="B149" s="1"/>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="1"/>
+      <c r="B150" s="1"/>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="1"/>
+      <c r="B152" s="1"/>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="1"/>
+      <c r="B153" s="1"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="1"/>
+      <c r="B154" s="1"/>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="1"/>
+      <c r="B155" s="1"/>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="1"/>
+      <c r="B156" s="1"/>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="1"/>
+      <c r="B157" s="1"/>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="1"/>
+      <c r="B158" s="1"/>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="1"/>
+      <c r="B159" s="1"/>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="1"/>
+      <c r="B160" s="1"/>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="1"/>
+      <c r="B165" s="1"/>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="1"/>
+      <c r="B168" s="1"/>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="1"/>
+      <c r="B177" s="1"/>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="1"/>
+      <c r="B179" s="1"/>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="1"/>
+      <c r="B180" s="1"/>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="1"/>
+      <c r="B182" s="1"/>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="1"/>
+      <c r="B183" s="1"/>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" s="1"/>
+      <c r="B184" s="1"/>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" s="1"/>
+      <c r="B185" s="1"/>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" s="1"/>
+      <c r="B186" s="1"/>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" s="1"/>
+      <c r="B187" s="1"/>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" s="1"/>
+      <c r="B188" s="1"/>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" s="1"/>
+      <c r="B189" s="1"/>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" s="1"/>
+      <c r="B190" s="1"/>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" s="1"/>
+      <c r="B191" s="1"/>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" s="1"/>
+      <c r="B192" s="1"/>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" s="1"/>
+      <c r="B193" s="1"/>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="1"/>
+      <c r="B194" s="1"/>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="1"/>
+      <c r="B195" s="1"/>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="1"/>
+      <c r="B196" s="1"/>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" s="1"/>
+      <c r="B197" s="1"/>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" s="1"/>
+      <c r="B198" s="1"/>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" s="1"/>
+      <c r="B199" s="1"/>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" s="1"/>
+      <c r="B200" s="1"/>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" s="1"/>
+      <c r="B201" s="1"/>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" s="1"/>
+      <c r="B202" s="1"/>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" s="1"/>
+      <c r="B203" s="1"/>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" s="1"/>
+      <c r="B204" s="1"/>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" s="1"/>
+      <c r="B205" s="1"/>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" s="1"/>
+      <c r="B206" s="1"/>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" s="1"/>
+      <c r="B207" s="1"/>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" s="1"/>
+      <c r="B208" s="1"/>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" s="1"/>
+      <c r="B209" s="1"/>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" s="1"/>
+      <c r="B210" s="1"/>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211" s="1"/>
+      <c r="B211" s="1"/>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212" s="1"/>
+      <c r="B212" s="1"/>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213" s="1"/>
+      <c r="B213" s="1"/>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214" s="1"/>
+      <c r="B214" s="1"/>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215" s="1"/>
+      <c r="B215" s="1"/>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216" s="1"/>
+      <c r="B216" s="1"/>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217" s="1"/>
+      <c r="B217" s="1"/>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" s="1"/>
+      <c r="B218" s="1"/>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219" s="1"/>
+      <c r="B219" s="1"/>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" s="1"/>
+      <c r="B220" s="1"/>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" s="1"/>
+      <c r="B221" s="1"/>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" s="1"/>
+      <c r="B222" s="1"/>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" s="1"/>
+      <c r="B223" s="1"/>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" s="1"/>
+      <c r="B224" s="1"/>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225" s="1"/>
+      <c r="B225" s="1"/>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226" s="1"/>
+      <c r="B226" s="1"/>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227" s="1"/>
+      <c r="B227" s="1"/>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228" s="1"/>
+      <c r="B228" s="1"/>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229" s="1"/>
+      <c r="B229" s="1"/>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230" s="1"/>
+      <c r="B230" s="1"/>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231" s="1"/>
+      <c r="B231" s="1"/>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232" s="1"/>
+      <c r="B232" s="1"/>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233" s="1"/>
+      <c r="B233" s="1"/>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234" s="1"/>
+      <c r="B234" s="1"/>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A235" s="1"/>
+      <c r="B235" s="1"/>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236" s="1"/>
+      <c r="B236" s="1"/>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237" s="1"/>
+      <c r="B237" s="1"/>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238" s="1"/>
+      <c r="B238" s="1"/>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239" s="1"/>
+      <c r="B239" s="1"/>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240" s="1"/>
+      <c r="B240" s="1"/>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241" s="1"/>
+      <c r="B241" s="1"/>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242" s="1"/>
+      <c r="B242" s="1"/>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A243" s="1"/>
+      <c r="B243" s="1"/>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244" s="1"/>
+      <c r="B244" s="1"/>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245" s="1"/>
+      <c r="B245" s="1"/>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246" s="1"/>
+      <c r="B246" s="1"/>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247" s="1"/>
+      <c r="B247" s="1"/>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248" s="1"/>
+      <c r="B248" s="1"/>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249" s="1"/>
+      <c r="B249" s="1"/>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250" s="1"/>
+      <c r="B250" s="1"/>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A251" s="1"/>
+      <c r="B251" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="A3:H10 B1:H1 B2:H2 H18:H251 C11 H11 C12 E12 H12 H13 H14 H15 H17" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>